<commit_message>
Se añade localizador dinamico en PaginaRegistro y se eliminan los localizadores instanciados en la clase Ingresar
</commit_message>
<xml_diff>
--- a/src/test/resources/data/data.xlsx
+++ b/src/test/resources/data/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspace\co.com.choucair.certification.utest\src\test\resources\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9860E57-2593-4813-90C1-57B488055076}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED61B15E-C266-4942-841D-A2701EB4BA20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -85,9 +85,6 @@
     <t>Linda</t>
   </si>
   <si>
-    <t>Perilla</t>
-  </si>
-  <si>
     <t>xyz@gmail.com</t>
   </si>
   <si>
@@ -115,9 +112,6 @@
     <t>iOS 12.0</t>
   </si>
   <si>
-    <t>Linda12345.</t>
-  </si>
-  <si>
     <t>CP002</t>
   </si>
   <si>
@@ -185,6 +179,12 @@
   </si>
   <si>
     <t>CP003</t>
+  </si>
+  <si>
+    <t>Choucair12345.</t>
+  </si>
+  <si>
+    <t>Fernandez</t>
   </si>
 </sst>
 </file>
@@ -539,7 +539,7 @@
   <dimension ref="A1:Q4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -622,19 +622,19 @@
         <v>18</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="1" t="s">
         <v>20</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>21</v>
       </c>
       <c r="F2" s="1">
         <v>110421</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H2" s="1">
         <v>5</v>
@@ -646,48 +646,48 @@
         <v>2002</v>
       </c>
       <c r="K2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="L2" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="M2" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="M2" s="1" t="s">
+      <c r="N2" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="N2" s="1" t="s">
+      <c r="O2" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="O2" s="1" t="s">
+      <c r="P2" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="P2" s="1" t="s">
-        <v>28</v>
-      </c>
       <c r="Q2" s="1" t="s">
-        <v>29</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>32</v>
-      </c>
       <c r="D3" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F3" s="1">
         <v>110421</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H3" s="1">
         <v>4</v>
@@ -699,48 +699,48 @@
         <v>1967</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="N3" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="P3" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="O3" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="P3" s="1" t="s">
-        <v>42</v>
-      </c>
       <c r="Q3" s="1" t="s">
-        <v>29</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F4" s="1">
         <v>110421</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H4" s="1">
         <v>7</v>
@@ -752,25 +752,25 @@
         <v>1973</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="M4" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="O4" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="N4" s="1" t="s">
+      <c r="P4" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="O4" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="P4" s="1" t="s">
-        <v>47</v>
-      </c>
       <c r="Q4" s="1" t="s">
-        <v>29</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -820,13 +820,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1" t="s">
         <v>33</v>
-      </c>
-      <c r="B1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C1" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>